<commit_message>
Notification number to be populated within the bulk template spreadsheet.
</commit_message>
<xml_diff>
--- a/src/EA.Iws.Api/Documents/BulkUploadPrenotificationTemplate.xlsx
+++ b/src/EA.Iws.Api/Documents/BulkUploadPrenotificationTemplate.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="http://teamshare1.ea.gov/directorates/EandB/IWSRFH/Shared Documents/IWS Online/3. BETA/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Source\EA\prsd-iws\src\EA.Iws.Api\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25200" windowHeight="11385" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25200" windowHeight="11385"/>
   </bookViews>
   <sheets>
     <sheet name="Prenotification TEMPLATE" sheetId="1" r:id="rId1"/>
@@ -88,7 +88,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -147,8 +147,36 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <dxfs count="2">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFD7D7D7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
+  <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
+    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
+      <tableStyleElement type="wholeTable" dxfId="1"/>
+      <tableStyleElement type="headerRow" dxfId="0"/>
+    </tableStyle>
+  </tableStyles>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -428,9 +456,9 @@
   </sheetPr>
   <dimension ref="A1:F1804"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozenSplit"/>
-      <selection pane="bottomLeft"/>
+      <selection pane="bottomLeft" activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -468,8 +496,6 @@
       <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="2"/>
-      <c r="E2" s="2"/>
       <c r="F2" s="2"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -9493,7 +9519,7 @@
   </sheetPr>
   <dimension ref="A1:F1805"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozenSplit"/>
       <selection pane="bottomLeft" activeCell="A11" sqref="A11:F14"/>
     </sheetView>
@@ -18775,20 +18801,20 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <Date xmlns="36541348-b42e-4df6-937f-59ca2d1235b1">2019-01-07T15:55:08+00:00</Date>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <Date xmlns="36541348-b42e-4df6-937f-59ca2d1235b1">2019-01-07T15:55:08+00:00</Date>
-  </documentManagement>
-</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -18810,14 +18836,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1EF24F8D-0333-44FC-8242-0F3262482854}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D7EA8666-8AEF-470F-B36A-6376BAE9B556}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
@@ -18831,4 +18849,12 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1EF24F8D-0333-44FC-8242-0F3262482854}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Bulk prenote updates (#724)
* Notification number to be populated within the bulk template spreadsheet.

* Add missing unit test for wrong notification number content validation.

* Fix issue with validating packaging types.

* Compare only the date values and ignore the time.

* Fix build error.
</commit_message>
<xml_diff>
--- a/src/EA.Iws.Api/Documents/BulkUploadPrenotificationTemplate.xlsx
+++ b/src/EA.Iws.Api/Documents/BulkUploadPrenotificationTemplate.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="http://teamshare1.ea.gov/directorates/EandB/IWSRFH/Shared Documents/IWS Online/3. BETA/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Source\EA\prsd-iws\src\EA.Iws.Api\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25200" windowHeight="11385" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25200" windowHeight="11385"/>
   </bookViews>
   <sheets>
     <sheet name="Prenotification TEMPLATE" sheetId="1" r:id="rId1"/>
@@ -88,7 +88,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -147,8 +147,36 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <dxfs count="2">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFD7D7D7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
+  <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
+    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
+      <tableStyleElement type="wholeTable" dxfId="1"/>
+      <tableStyleElement type="headerRow" dxfId="0"/>
+    </tableStyle>
+  </tableStyles>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -428,9 +456,9 @@
   </sheetPr>
   <dimension ref="A1:F1804"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozenSplit"/>
-      <selection pane="bottomLeft"/>
+      <selection pane="bottomLeft" activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -468,8 +496,6 @@
       <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="2"/>
-      <c r="E2" s="2"/>
       <c r="F2" s="2"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -9493,7 +9519,7 @@
   </sheetPr>
   <dimension ref="A1:F1805"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozenSplit"/>
       <selection pane="bottomLeft" activeCell="A11" sqref="A11:F14"/>
     </sheetView>
@@ -18775,20 +18801,20 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <Date xmlns="36541348-b42e-4df6-937f-59ca2d1235b1">2019-01-07T15:55:08+00:00</Date>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <Date xmlns="36541348-b42e-4df6-937f-59ca2d1235b1">2019-01-07T15:55:08+00:00</Date>
-  </documentManagement>
-</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -18810,14 +18836,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1EF24F8D-0333-44FC-8242-0F3262482854}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D7EA8666-8AEF-470F-B36A-6376BAE9B556}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
@@ -18831,4 +18849,12 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1EF24F8D-0333-44FC-8242-0F3262482854}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Updated text as per bug 67129
</commit_message>
<xml_diff>
--- a/src/EA.Iws.Api/Documents/BulkUploadPrenotificationTemplate.xlsx
+++ b/src/EA.Iws.Api/Documents/BulkUploadPrenotificationTemplate.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Source\EA\prsd-iws\src\EA.Iws.Api\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Repos\EnvironmentAgency\prsd-iws\src\EA.Iws.Api\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -70,9 +70,6 @@
     <t>This is a numerical field and must contain whole numbers. The number must be the shipment number of the prenotification</t>
   </si>
   <si>
-    <t>This column should be in a numerical format; no more than 4 decimal places</t>
-  </si>
-  <si>
     <t>This is a textual field. The unit of measurement must be written as, for example, Tonnes or m3</t>
   </si>
   <si>
@@ -84,11 +81,14 @@
   <si>
     <t>An example is provided below</t>
   </si>
+  <si>
+    <t>This column must be in a numerical format; no more than 4 decimal places</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -458,7 +458,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozenSplit"/>
-      <selection pane="bottomLeft" activeCell="E2" sqref="E2"/>
+      <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9521,7 +9521,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozenSplit"/>
-      <selection pane="bottomLeft" activeCell="A11" sqref="A11:F14"/>
+      <selection pane="bottomLeft" activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9543,13 +9543,13 @@
         <v>12</v>
       </c>
       <c r="C1" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="D1" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="E1" s="4" t="s">
         <v>14</v>
-      </c>
-      <c r="E1" s="4" t="s">
-        <v>15</v>
       </c>
       <c r="F1" s="4" t="s">
         <v>4</v>
@@ -9565,7 +9565,7 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -9680,7 +9680,7 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B11" s="5"/>
       <c r="C11" s="5"/>
@@ -18675,6 +18675,23 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <Date xmlns="36541348-b42e-4df6-937f-59ca2d1235b1">2019-01-07T15:55:08+00:00</Date>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101007759CA8CE08AB9419CDC954FF1613187" ma:contentTypeVersion="" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="471c13ecf6b8d239f1a9ed47c0d50475">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="36541348-b42e-4df6-937f-59ca2d1235b1" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="199054d83c20ad432576f091e08ce527" ns2:_="">
     <xsd:import namespace="36541348-b42e-4df6-937f-59ca2d1235b1"/>
@@ -18800,37 +18817,10 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <Date xmlns="36541348-b42e-4df6-937f-59ca2d1235b1">2019-01-07T15:55:08+00:00</Date>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CF4FA9BA-83C9-4F54-BCD2-16BFAE0A66D3}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1EF24F8D-0333-44FC-8242-0F3262482854}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="36541348-b42e-4df6-937f-59ca2d1235b1"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -18852,9 +18842,19 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1EF24F8D-0333-44FC-8242-0F3262482854}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CF4FA9BA-83C9-4F54-BCD2-16BFAE0A66D3}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="36541348-b42e-4df6-937f-59ca2d1235b1"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Updated text as per bug 67129 (#745)
</commit_message>
<xml_diff>
--- a/src/EA.Iws.Api/Documents/BulkUploadPrenotificationTemplate.xlsx
+++ b/src/EA.Iws.Api/Documents/BulkUploadPrenotificationTemplate.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Source\EA\prsd-iws\src\EA.Iws.Api\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Repos\EnvironmentAgency\prsd-iws\src\EA.Iws.Api\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -70,9 +70,6 @@
     <t>This is a numerical field and must contain whole numbers. The number must be the shipment number of the prenotification</t>
   </si>
   <si>
-    <t>This column should be in a numerical format; no more than 4 decimal places</t>
-  </si>
-  <si>
     <t>This is a textual field. The unit of measurement must be written as, for example, Tonnes or m3</t>
   </si>
   <si>
@@ -84,11 +81,14 @@
   <si>
     <t>An example is provided below</t>
   </si>
+  <si>
+    <t>This column must be in a numerical format; no more than 4 decimal places</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -458,7 +458,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozenSplit"/>
-      <selection pane="bottomLeft" activeCell="E2" sqref="E2"/>
+      <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9521,7 +9521,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozenSplit"/>
-      <selection pane="bottomLeft" activeCell="A11" sqref="A11:F14"/>
+      <selection pane="bottomLeft" activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9543,13 +9543,13 @@
         <v>12</v>
       </c>
       <c r="C1" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="D1" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="E1" s="4" t="s">
         <v>14</v>
-      </c>
-      <c r="E1" s="4" t="s">
-        <v>15</v>
       </c>
       <c r="F1" s="4" t="s">
         <v>4</v>
@@ -9565,7 +9565,7 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -9680,7 +9680,7 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B11" s="5"/>
       <c r="C11" s="5"/>
@@ -18675,6 +18675,23 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <Date xmlns="36541348-b42e-4df6-937f-59ca2d1235b1">2019-01-07T15:55:08+00:00</Date>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101007759CA8CE08AB9419CDC954FF1613187" ma:contentTypeVersion="" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="471c13ecf6b8d239f1a9ed47c0d50475">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="36541348-b42e-4df6-937f-59ca2d1235b1" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="199054d83c20ad432576f091e08ce527" ns2:_="">
     <xsd:import namespace="36541348-b42e-4df6-937f-59ca2d1235b1"/>
@@ -18800,37 +18817,10 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <Date xmlns="36541348-b42e-4df6-937f-59ca2d1235b1">2019-01-07T15:55:08+00:00</Date>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CF4FA9BA-83C9-4F54-BCD2-16BFAE0A66D3}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1EF24F8D-0333-44FC-8242-0F3262482854}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="36541348-b42e-4df6-937f-59ca2d1235b1"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -18852,9 +18842,19 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1EF24F8D-0333-44FC-8242-0F3262482854}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CF4FA9BA-83C9-4F54-BCD2-16BFAE0A66D3}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="36541348-b42e-4df6-937f-59ca2d1235b1"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Update text on template guidance sheet regarding decimals.
</commit_message>
<xml_diff>
--- a/src/EA.Iws.Api/Documents/BulkUploadPrenotificationTemplate.xlsx
+++ b/src/EA.Iws.Api/Documents/BulkUploadPrenotificationTemplate.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Repos\EnvironmentAgency\prsd-iws\src\EA.Iws.Api\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Source\EA\prsd-iws\src\EA.Iws.Api\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25200" windowHeight="11385"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25200" windowHeight="11385" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Prenotification TEMPLATE" sheetId="1" r:id="rId1"/>
@@ -82,13 +82,13 @@
     <t>An example is provided below</t>
   </si>
   <si>
-    <t>This column must be in a numerical format; no more than 4 decimal places</t>
+    <t>This column must be in a numerical format; no more than 4 decimal places for measurements in Tonnes or 1 decimal place for measurements in Kilograms</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -456,7 +456,7 @@
   </sheetPr>
   <dimension ref="A1:F1804"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozenSplit"/>
       <selection pane="bottomLeft"/>
     </sheetView>
@@ -9519,9 +9519,9 @@
   </sheetPr>
   <dimension ref="A1:F1805"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozenSplit"/>
-      <selection pane="bottomLeft" activeCell="C2" sqref="C2"/>
+      <selection pane="bottomLeft" activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9535,7 +9535,7 @@
     <col min="7" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" ht="135" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>11</v>
       </c>
@@ -18684,14 +18684,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <Date xmlns="36541348-b42e-4df6-937f-59ca2d1235b1">2019-01-07T15:55:08+00:00</Date>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101007759CA8CE08AB9419CDC954FF1613187" ma:contentTypeVersion="" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="471c13ecf6b8d239f1a9ed47c0d50475">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="36541348-b42e-4df6-937f-59ca2d1235b1" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="199054d83c20ad432576f091e08ce527" ns2:_="">
     <xsd:import namespace="36541348-b42e-4df6-937f-59ca2d1235b1"/>
@@ -18817,6 +18809,14 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <Date xmlns="36541348-b42e-4df6-937f-59ca2d1235b1">2019-01-07T15:55:08+00:00</Date>
+  </documentManagement>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1EF24F8D-0333-44FC-8242-0F3262482854}">
   <ds:schemaRefs>
@@ -18826,22 +18826,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D7EA8666-8AEF-470F-B36A-6376BAE9B556}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="36541348-b42e-4df6-937f-59ca2d1235b1"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CF4FA9BA-83C9-4F54-BCD2-16BFAE0A66D3}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -18857,4 +18841,20 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D7EA8666-8AEF-470F-B36A-6376BAE9B556}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="36541348-b42e-4df6-937f-59ca2d1235b1"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Update text on template guidance sheet regarding decimals. (#772)
</commit_message>
<xml_diff>
--- a/src/EA.Iws.Api/Documents/BulkUploadPrenotificationTemplate.xlsx
+++ b/src/EA.Iws.Api/Documents/BulkUploadPrenotificationTemplate.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Repos\EnvironmentAgency\prsd-iws\src\EA.Iws.Api\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Source\EA\prsd-iws\src\EA.Iws.Api\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25200" windowHeight="11385"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25200" windowHeight="11385" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Prenotification TEMPLATE" sheetId="1" r:id="rId1"/>
@@ -82,13 +82,13 @@
     <t>An example is provided below</t>
   </si>
   <si>
-    <t>This column must be in a numerical format; no more than 4 decimal places</t>
+    <t>This column must be in a numerical format; no more than 4 decimal places for measurements in Tonnes or 1 decimal place for measurements in Kilograms</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -456,7 +456,7 @@
   </sheetPr>
   <dimension ref="A1:F1804"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozenSplit"/>
       <selection pane="bottomLeft"/>
     </sheetView>
@@ -9519,9 +9519,9 @@
   </sheetPr>
   <dimension ref="A1:F1805"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozenSplit"/>
-      <selection pane="bottomLeft" activeCell="C2" sqref="C2"/>
+      <selection pane="bottomLeft" activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9535,7 +9535,7 @@
     <col min="7" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" ht="135" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>11</v>
       </c>
@@ -18684,14 +18684,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <Date xmlns="36541348-b42e-4df6-937f-59ca2d1235b1">2019-01-07T15:55:08+00:00</Date>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101007759CA8CE08AB9419CDC954FF1613187" ma:contentTypeVersion="" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="471c13ecf6b8d239f1a9ed47c0d50475">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="36541348-b42e-4df6-937f-59ca2d1235b1" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="199054d83c20ad432576f091e08ce527" ns2:_="">
     <xsd:import namespace="36541348-b42e-4df6-937f-59ca2d1235b1"/>
@@ -18817,6 +18809,14 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <Date xmlns="36541348-b42e-4df6-937f-59ca2d1235b1">2019-01-07T15:55:08+00:00</Date>
+  </documentManagement>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1EF24F8D-0333-44FC-8242-0F3262482854}">
   <ds:schemaRefs>
@@ -18826,22 +18826,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D7EA8666-8AEF-470F-B36A-6376BAE9B556}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="36541348-b42e-4df6-937f-59ca2d1235b1"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CF4FA9BA-83C9-4F54-BCD2-16BFAE0A66D3}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -18857,4 +18841,20 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D7EA8666-8AEF-470F-B36A-6376BAE9B556}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="36541348-b42e-4df6-937f-59ca2d1235b1"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Update text on guidance sheet for bulk prenotes.
</commit_message>
<xml_diff>
--- a/src/EA.Iws.Api/Documents/BulkUploadPrenotificationTemplate.xlsx
+++ b/src/EA.Iws.Api/Documents/BulkUploadPrenotificationTemplate.xlsx
@@ -64,9 +64,6 @@
     <t>Actual Date of Shipment</t>
   </si>
   <si>
-    <t>This is a textual field and will contain the notification number with no blank spaces</t>
-  </si>
-  <si>
     <t>This is a numerical field and must contain whole numbers. The number must be the shipment number of the prenotification</t>
   </si>
   <si>
@@ -83,6 +80,9 @@
   </si>
   <si>
     <t>This column must be in a numerical format; no more than 4 decimal places for measurements in Tonnes or 1 decimal place for measurements in Kilograms</t>
+  </si>
+  <si>
+    <t>This is a textual field and will contain the notification number</t>
   </si>
 </sst>
 </file>
@@ -9521,7 +9521,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozenSplit"/>
-      <selection pane="bottomLeft" activeCell="C8" sqref="C8"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9537,19 +9537,19 @@
   <sheetData>
     <row r="1" spans="1:6" ht="135" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B1" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="C1" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="D1" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="C1" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="D1" s="4" t="s">
+      <c r="E1" s="4" t="s">
         <v>13</v>
-      </c>
-      <c r="E1" s="4" t="s">
-        <v>14</v>
       </c>
       <c r="F1" s="4" t="s">
         <v>4</v>
@@ -9565,7 +9565,7 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -9680,7 +9680,7 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B11" s="5"/>
       <c r="C11" s="5"/>
@@ -18684,6 +18684,14 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <Date xmlns="36541348-b42e-4df6-937f-59ca2d1235b1">2019-01-07T15:55:08+00:00</Date>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101007759CA8CE08AB9419CDC954FF1613187" ma:contentTypeVersion="" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="471c13ecf6b8d239f1a9ed47c0d50475">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="36541348-b42e-4df6-937f-59ca2d1235b1" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="199054d83c20ad432576f091e08ce527" ns2:_="">
     <xsd:import namespace="36541348-b42e-4df6-937f-59ca2d1235b1"/>
@@ -18809,14 +18817,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <Date xmlns="36541348-b42e-4df6-937f-59ca2d1235b1">2019-01-07T15:55:08+00:00</Date>
-  </documentManagement>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1EF24F8D-0333-44FC-8242-0F3262482854}">
   <ds:schemaRefs>
@@ -18826,6 +18826,22 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D7EA8666-8AEF-470F-B36A-6376BAE9B556}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="36541348-b42e-4df6-937f-59ca2d1235b1"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CF4FA9BA-83C9-4F54-BCD2-16BFAE0A66D3}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -18841,20 +18857,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D7EA8666-8AEF-470F-B36A-6376BAE9B556}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="36541348-b42e-4df6-937f-59ca2d1235b1"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>